<commit_message>
Update Usecase Format, Activity Quản lí đặt hàng, hóa đơn
</commit_message>
<xml_diff>
--- a/Thiết kế/UseCases/7. Đặt hàng + 8. Hoá đơn.xlsx
+++ b/Thiết kế/UseCases/7. Đặt hàng + 8. Hoá đơn.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CNPM\Thiết kế\UseCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Homework\CN Phan Mem\Homework\CNPM\Thiết kế\UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC241DEC-A096-4CD6-A2FC-3175A5A4123E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AFFD58-525B-4D8C-86DA-9F090589F7F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Quản lí đặt hàng" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="77">
   <si>
     <t>Use Case Number:</t>
   </si>
@@ -148,12 +148,6 @@
     <t>4. Hệ thống hiển thị cửa sổ cập nhật</t>
   </si>
   <si>
-    <t>5. Actor nhập thông tin sau đó bấm cấp nhật</t>
-  </si>
-  <si>
-    <t>6. Hệ thống lưu các thay đổi mới vào cơ sở dữ liệu, báo cập nhật thành công.</t>
-  </si>
-  <si>
     <t>A3.</t>
   </si>
   <si>
@@ -163,30 +157,7 @@
     <t>2. Quay về bước 4</t>
   </si>
   <si>
-    <t xml:space="preserve">A4. </t>
-  </si>
-  <si>
     <t>Thủ kho, máy in</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">9. Hệ thống lưu vào cơ sở dữ liệu và hiển thị đơn đặt hàng vừa tạo. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>A4</t>
-    </r>
-  </si>
-  <si>
-    <t>1. Actor nhấn nút in</t>
-  </si>
-  <si>
-    <t>2. Hệ thống in đơn đặt hàng bằng máy in</t>
   </si>
   <si>
     <t>Exception Paths:</t>
@@ -285,9 +256,6 @@
     <t>4. Hệ thống truy cập cơ sở dữ liệu sản phẩm hiển thị cửa sổ tạo hoá đơn</t>
   </si>
   <si>
-    <t>9. Hệ thống lưu hoá đơn vào cơ sở dữ liệu và in hoá đơn qua máy in</t>
-  </si>
-  <si>
     <t>Nhân viên bán hàng, máy in</t>
   </si>
   <si>
@@ -317,9 +285,6 @@
     <t>5. Actor nhập thông tin mới và bấm cập nhật</t>
   </si>
   <si>
-    <t>6. Hệ thống lưu vào cơ sở dữ liệu và báo cập nhật thành công</t>
-  </si>
-  <si>
     <t>1. Hệ thống không tìm được khách hàng trong cơ sở dữ liệu</t>
   </si>
   <si>
@@ -358,7 +323,44 @@
     <t>Actor đã đăng nhập và có quyền sử dụng chức năng</t>
   </si>
   <si>
-    <t>3. Actor xem cửa sổ đã hiển thị. Use Case kết thúc tại đây</t>
+    <t>9. Hệ thống lưu hoá đơn vào cơ sở dữ liệu và in hoá đơn qua máy in, use case kết thúc tại đây.</t>
+  </si>
+  <si>
+    <t>2. Hệ thống hiển thị chi tiết hoá đơn vừa chọn. Use case kết thúc tại đây</t>
+  </si>
+  <si>
+    <t>6. Hệ thống lưu vào cơ sở dữ liệu và báo cập nhật thành công, use case kết thúc tại đây.</t>
+  </si>
+  <si>
+    <t>6. Hệ thống lưu các thay đổi mới vào cơ sở dữ liệu, báo cập nhật thành công. Use case kết thúc tại đây</t>
+  </si>
+  <si>
+    <t>2. Hệ thống hiển thị cửa sổ thông tin đơn hàng. Use Case kết thúc tại đây</t>
+  </si>
+  <si>
+    <t>5. Actor nhập thông tin sau đó bấm cập nhật</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9. Hệ thống lưu vào cơ sở dữ liệu và hiển thị đơn đặt hàng vừa tạo. Use case kết thúc tại đây. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>A4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>. Actor chọn hủy, quay về bước 4 của A2.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -393,7 +395,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -453,11 +455,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -480,6 +508,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -491,6 +525,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -515,21 +555,21 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>324831</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>86965</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>252630</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>395149</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DEB92D1-216C-4444-AB04-45840F9E1C45}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02FBFE1A-7140-41D8-B66D-7323A9F58B15}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -545,8 +585,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8220075" y="0"/>
-          <a:ext cx="7030431" cy="8888065"/>
+          <a:off x="8442960" y="213360"/>
+          <a:ext cx="5876190" cy="8723809"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -564,21 +604,21 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>20074</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>39334</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>18340</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>132425</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61B65A8E-4F63-4B0F-A714-28D2F2788ADE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6943E55-FE7A-4343-BB49-CD593AD594F5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -594,8 +634,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8353425" y="0"/>
-          <a:ext cx="7335274" cy="8840434"/>
+          <a:off x="8591550" y="209550"/>
+          <a:ext cx="5676190" cy="7400000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -870,66 +910,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C85"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" style="2" customWidth="1"/>
-    <col min="2" max="3" width="39.7109375" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="34.6640625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="39.6640625" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8"/>
-    </row>
-    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C2" s="10"/>
+    </row>
+    <row r="3" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="8"/>
-    </row>
-    <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="10"/>
+    </row>
+    <row r="4" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8"/>
-    </row>
-    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="8"/>
-    </row>
-    <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -939,85 +979,85 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+    <row r="7" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="9"/>
       <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+    <row r="8" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+    <row r="9" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
       <c r="B9" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+    <row r="10" spans="1:3" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="9"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+    <row r="11" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
       <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+    <row r="12" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+    <row r="13" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="9"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="66" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+    <row r="14" spans="1:3" ht="67.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="9"/>
       <c r="B14" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+    <row r="15" spans="1:3" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="9"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-    </row>
-    <row r="17" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+    </row>
+    <row r="17" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="8"/>
-    </row>
-    <row r="18" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="C17" s="10"/>
+    </row>
+    <row r="18" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="12"/>
       <c r="B18" s="5" t="s">
         <v>10</v>
       </c>
@@ -1025,448 +1065,412 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+    <row r="19" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="12"/>
       <c r="B19" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="6"/>
     </row>
-    <row r="20" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+    <row r="20" spans="1:3" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="12"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="12"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+    </row>
+    <row r="22" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="12"/>
+      <c r="B22" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="10"/>
+    </row>
+    <row r="23" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="12"/>
+      <c r="B24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="12"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-    </row>
-    <row r="23" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="8"/>
-    </row>
-    <row r="24" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="5" t="s">
+    <row r="26" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="12"/>
+      <c r="B26" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="12"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="12"/>
+      <c r="B28" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:3" ht="67.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="12"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="12"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+    </row>
+    <row r="31" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="12"/>
+      <c r="B31" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="10"/>
+    </row>
+    <row r="32" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="12"/>
+      <c r="B32" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C32" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="6"/>
-    </row>
-    <row r="26" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6" t="s">
+    <row r="33" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="12"/>
+      <c r="B33" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-    </row>
-    <row r="32" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7" t="s">
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="13"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="8"/>
-    </row>
-    <row r="33" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="6"/>
-    </row>
-    <row r="35" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6" t="s">
+    </row>
+    <row r="35" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="8"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="15"/>
+    </row>
+    <row r="36" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+      <c r="B36" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="10"/>
+    </row>
+    <row r="37" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-    </row>
-    <row r="37" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="8"/>
-    </row>
-    <row r="38" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="6" t="s">
+      <c r="C37" s="10"/>
+    </row>
+    <row r="38" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="10"/>
+    </row>
+    <row r="39" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="10"/>
+    </row>
+    <row r="40" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="6"/>
-    </row>
-    <row r="40" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6" t="s">
+      <c r="B40" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="10"/>
+    </row>
+    <row r="41" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-    </row>
-    <row r="42" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B41" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="10"/>
+    </row>
+    <row r="42" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="10"/>
+    </row>
+    <row r="43" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="8"/>
-    </row>
-    <row r="43" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+      <c r="B43" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" s="10"/>
+    </row>
+    <row r="44" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C43" s="8"/>
-    </row>
-    <row r="44" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+      <c r="B44" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" s="10"/>
+    </row>
+    <row r="45" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C44" s="8"/>
-    </row>
-    <row r="45" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C45" s="8"/>
-    </row>
-    <row r="46" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" s="8"/>
-    </row>
-    <row r="47" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C47" s="8"/>
-    </row>
-    <row r="48" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C48" s="8"/>
-    </row>
-    <row r="49" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+      <c r="B45" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B49" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C49" s="8"/>
-    </row>
-    <row r="50" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C50" s="8"/>
-    </row>
-    <row r="51" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C45" s="10"/>
+    </row>
+    <row r="46" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46"/>
+      <c r="B46"/>
+      <c r="C46"/>
+    </row>
+    <row r="47" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47"/>
+      <c r="B47"/>
+      <c r="C47"/>
+    </row>
+    <row r="48" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48"/>
+      <c r="B48"/>
+      <c r="C48"/>
+    </row>
+    <row r="49" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49"/>
+      <c r="B49"/>
+      <c r="C49"/>
+    </row>
+    <row r="50" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50"/>
+      <c r="B50"/>
+      <c r="C50"/>
+    </row>
+    <row r="51" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51"/>
       <c r="B51"/>
       <c r="C51"/>
     </row>
-    <row r="52" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52"/>
     </row>
-    <row r="53" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53"/>
     </row>
-    <row r="54" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54"/>
     </row>
-    <row r="55" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55"/>
       <c r="B55"/>
       <c r="C55"/>
     </row>
-    <row r="56" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56"/>
     </row>
-    <row r="57" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57"/>
       <c r="B57"/>
       <c r="C57"/>
     </row>
-    <row r="58" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
     </row>
-    <row r="59" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59"/>
     </row>
-    <row r="60" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
     </row>
-    <row r="61" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61"/>
       <c r="B61"/>
       <c r="C61"/>
     </row>
-    <row r="62" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62"/>
       <c r="B62"/>
       <c r="C62"/>
     </row>
-    <row r="63" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63"/>
     </row>
-    <row r="64" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64"/>
       <c r="B64"/>
       <c r="C64"/>
     </row>
-    <row r="65" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65"/>
       <c r="B65"/>
       <c r="C65"/>
     </row>
-    <row r="66" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66"/>
       <c r="B66"/>
       <c r="C66"/>
     </row>
-    <row r="67" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67"/>
       <c r="B67"/>
       <c r="C67"/>
     </row>
-    <row r="68" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68"/>
       <c r="B68"/>
       <c r="C68"/>
     </row>
-    <row r="69" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69"/>
       <c r="B69"/>
       <c r="C69"/>
     </row>
-    <row r="70" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70"/>
       <c r="B70"/>
       <c r="C70"/>
     </row>
-    <row r="71" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71"/>
       <c r="B71"/>
       <c r="C71"/>
     </row>
-    <row r="72" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72"/>
       <c r="B72"/>
       <c r="C72"/>
     </row>
-    <row r="73" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73"/>
       <c r="B73"/>
       <c r="C73"/>
     </row>
-    <row r="74" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74"/>
       <c r="B74"/>
       <c r="C74"/>
     </row>
-    <row r="75" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75"/>
       <c r="B75"/>
       <c r="C75"/>
     </row>
-    <row r="76" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76"/>
       <c r="B76"/>
       <c r="C76"/>
     </row>
-    <row r="77" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77"/>
       <c r="B77"/>
       <c r="C77"/>
     </row>
-    <row r="78" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78"/>
       <c r="B78"/>
       <c r="C78"/>
     </row>
-    <row r="79" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79"/>
       <c r="B79"/>
       <c r="C79"/>
     </row>
-    <row r="80" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80"/>
       <c r="B80"/>
       <c r="C80"/>
     </row>
-    <row r="81" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81"/>
-      <c r="B81"/>
-      <c r="C81"/>
-    </row>
-    <row r="82" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82"/>
-      <c r="B82"/>
-      <c r="C82"/>
-    </row>
-    <row r="83" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83"/>
-      <c r="B83"/>
-      <c r="C83"/>
-    </row>
-    <row r="84" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84"/>
-      <c r="B84"/>
-      <c r="C84"/>
-    </row>
-    <row r="85" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85"/>
-      <c r="B85"/>
-      <c r="C85"/>
-    </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="A17:A40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B31:C31"/>
+  <mergeCells count="24">
     <mergeCell ref="A6:A15"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A17:A34"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1478,1048 +1482,1046 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2245BF36-93D6-4E8F-9084-C70B43C0A7D9}">
   <dimension ref="A1:C178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" style="2" customWidth="1"/>
-    <col min="2" max="3" width="40.7109375" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="34.6640625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="40.6640625" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="8"/>
-    </row>
-    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="10"/>
+    </row>
+    <row r="3" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="8"/>
-    </row>
-    <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="10"/>
+    </row>
+    <row r="4" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8"/>
-    </row>
-    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="8"/>
-    </row>
-    <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="B5" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+    <row r="7" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="9"/>
       <c r="B7" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+    <row r="8" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+    <row r="9" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
       <c r="B9" s="4" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+    <row r="10" spans="1:3" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="9"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
       <c r="B11" s="4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+    <row r="12" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="9"/>
       <c r="B13" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3" ht="66" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+    <row r="14" spans="1:3" ht="67.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="9"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="9"/>
       <c r="B15" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+    <row r="16" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="9"/>
       <c r="B16" s="4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+    <row r="17" spans="1:3" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="9"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-    </row>
-    <row r="19" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+    </row>
+    <row r="19" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="7"/>
-    </row>
-    <row r="20" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="4" t="s">
+      <c r="C19" s="9"/>
+    </row>
+    <row r="20" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="12"/>
+      <c r="B20" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
+    <row r="21" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="12"/>
       <c r="B21" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
+    <row r="22" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="12"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-    </row>
-    <row r="24" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+    </row>
+    <row r="24" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="12"/>
+      <c r="B24" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="8"/>
-    </row>
-    <row r="25" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="4" t="s">
+      <c r="C24" s="10"/>
+    </row>
+    <row r="25" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="12"/>
+      <c r="B25" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
+    <row r="26" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="12"/>
       <c r="B26" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
+    <row r="27" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="12"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="12"/>
       <c r="B28" s="4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
+    <row r="29" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="12"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
+    <row r="30" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="12"/>
       <c r="B30" s="4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
+    <row r="31" spans="1:3" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="12"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-    </row>
-    <row r="33" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="8"/>
-    </row>
-    <row r="34" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="12"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+    </row>
+    <row r="33" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="12"/>
+      <c r="B33" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="10"/>
+    </row>
+    <row r="34" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="12"/>
+      <c r="B34" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
+    <row r="35" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="12"/>
       <c r="B35" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
+    <row r="36" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="13"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+    </row>
+    <row r="38" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="11" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-    </row>
-    <row r="38" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C38" s="7"/>
-    </row>
-    <row r="39" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="10"/>
-      <c r="B39" s="4" t="s">
+      <c r="B38" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="9"/>
+    </row>
+    <row r="39" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="12"/>
+      <c r="B39" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
+    <row r="40" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="12"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="12"/>
       <c r="B41" s="4" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
+    <row r="42" spans="1:3" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="13"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" s="10"/>
+    </row>
+    <row r="44" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C44" s="10"/>
+    </row>
+    <row r="45" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" s="10"/>
+    </row>
+    <row r="46" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C46" s="10"/>
+    </row>
+    <row r="47" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47" s="10"/>
+    </row>
+    <row r="48" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" s="10"/>
+    </row>
+    <row r="49" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C43" s="8"/>
-    </row>
-    <row r="44" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="B49" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49" s="10"/>
+    </row>
+    <row r="50" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" s="8"/>
-    </row>
-    <row r="45" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C45" s="8"/>
-    </row>
-    <row r="46" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C46" s="8"/>
-    </row>
-    <row r="47" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C47" s="8"/>
-    </row>
-    <row r="48" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C48" s="8"/>
-    </row>
-    <row r="49" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="B50" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B49" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C49" s="8"/>
-    </row>
-    <row r="50" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C50" s="8"/>
-    </row>
-    <row r="51" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C50" s="10"/>
+    </row>
+    <row r="51" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51"/>
       <c r="B51"/>
       <c r="C51"/>
     </row>
-    <row r="52" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52"/>
     </row>
-    <row r="53" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53"/>
     </row>
-    <row r="54" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54"/>
     </row>
-    <row r="55" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55"/>
       <c r="B55"/>
       <c r="C55"/>
     </row>
-    <row r="56" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56"/>
     </row>
-    <row r="57" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57"/>
       <c r="B57"/>
       <c r="C57"/>
     </row>
-    <row r="58" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
     </row>
-    <row r="59" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59"/>
     </row>
-    <row r="60" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
     </row>
-    <row r="61" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61"/>
       <c r="B61"/>
       <c r="C61"/>
     </row>
-    <row r="62" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62"/>
       <c r="B62"/>
       <c r="C62"/>
     </row>
-    <row r="63" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63"/>
     </row>
-    <row r="64" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64"/>
       <c r="B64"/>
       <c r="C64"/>
     </row>
-    <row r="65" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65"/>
       <c r="B65"/>
       <c r="C65"/>
     </row>
-    <row r="66" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66"/>
       <c r="B66"/>
       <c r="C66"/>
     </row>
-    <row r="67" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67"/>
       <c r="B67"/>
       <c r="C67"/>
     </row>
-    <row r="68" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68"/>
       <c r="B68"/>
       <c r="C68"/>
     </row>
-    <row r="69" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69"/>
       <c r="B69"/>
       <c r="C69"/>
     </row>
-    <row r="70" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70"/>
       <c r="B70"/>
       <c r="C70"/>
     </row>
-    <row r="71" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71"/>
       <c r="B71"/>
       <c r="C71"/>
     </row>
-    <row r="72" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72"/>
       <c r="B72"/>
       <c r="C72"/>
     </row>
-    <row r="73" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73"/>
       <c r="B73"/>
       <c r="C73"/>
     </row>
-    <row r="74" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74"/>
       <c r="B74"/>
       <c r="C74"/>
     </row>
-    <row r="75" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75"/>
       <c r="B75"/>
       <c r="C75"/>
     </row>
-    <row r="76" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76"/>
       <c r="B76"/>
       <c r="C76"/>
     </row>
-    <row r="77" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77"/>
       <c r="B77"/>
       <c r="C77"/>
     </row>
-    <row r="78" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78"/>
       <c r="B78"/>
       <c r="C78"/>
     </row>
-    <row r="79" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79"/>
       <c r="B79"/>
       <c r="C79"/>
     </row>
-    <row r="80" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80"/>
       <c r="B80"/>
       <c r="C80"/>
     </row>
-    <row r="81" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81"/>
       <c r="B81"/>
       <c r="C81"/>
     </row>
-    <row r="82" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82"/>
       <c r="B82"/>
       <c r="C82"/>
     </row>
-    <row r="83" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83"/>
       <c r="B83"/>
       <c r="C83"/>
     </row>
-    <row r="84" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84"/>
       <c r="B84"/>
       <c r="C84"/>
     </row>
-    <row r="85" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85"/>
       <c r="B85"/>
       <c r="C85"/>
     </row>
-    <row r="86" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86"/>
       <c r="B86"/>
       <c r="C86"/>
     </row>
-    <row r="87" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87"/>
       <c r="B87"/>
       <c r="C87"/>
     </row>
-    <row r="88" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88"/>
       <c r="B88"/>
       <c r="C88"/>
     </row>
-    <row r="89" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89"/>
       <c r="B89"/>
       <c r="C89"/>
     </row>
-    <row r="90" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90"/>
       <c r="B90"/>
       <c r="C90"/>
     </row>
-    <row r="91" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91"/>
       <c r="B91"/>
       <c r="C91"/>
     </row>
-    <row r="92" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92"/>
       <c r="B92"/>
       <c r="C92"/>
     </row>
-    <row r="93" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93"/>
       <c r="B93"/>
       <c r="C93"/>
     </row>
-    <row r="94" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94"/>
       <c r="B94"/>
       <c r="C94"/>
     </row>
-    <row r="95" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95"/>
       <c r="B95"/>
       <c r="C95"/>
     </row>
-    <row r="96" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96"/>
       <c r="B96"/>
       <c r="C96"/>
     </row>
-    <row r="97" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97"/>
       <c r="B97"/>
       <c r="C97"/>
     </row>
-    <row r="98" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98"/>
       <c r="B98"/>
       <c r="C98"/>
     </row>
-    <row r="99" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99"/>
       <c r="B99"/>
       <c r="C99"/>
     </row>
-    <row r="100" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100"/>
       <c r="B100"/>
       <c r="C100"/>
     </row>
-    <row r="101" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101"/>
       <c r="B101"/>
       <c r="C101"/>
     </row>
-    <row r="102" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102"/>
       <c r="B102"/>
       <c r="C102"/>
     </row>
-    <row r="103" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103"/>
       <c r="B103"/>
       <c r="C103"/>
     </row>
-    <row r="104" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104"/>
       <c r="B104"/>
       <c r="C104"/>
     </row>
-    <row r="105" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105"/>
       <c r="B105"/>
       <c r="C105"/>
     </row>
-    <row r="106" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106"/>
       <c r="B106"/>
       <c r="C106"/>
     </row>
-    <row r="107" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107"/>
       <c r="B107"/>
       <c r="C107"/>
     </row>
-    <row r="108" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108"/>
       <c r="B108"/>
       <c r="C108"/>
     </row>
-    <row r="109" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109"/>
       <c r="B109"/>
       <c r="C109"/>
     </row>
-    <row r="110" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110"/>
       <c r="B110"/>
       <c r="C110"/>
     </row>
-    <row r="111" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111"/>
       <c r="B111"/>
       <c r="C111"/>
     </row>
-    <row r="112" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112"/>
       <c r="B112"/>
       <c r="C112"/>
     </row>
-    <row r="113" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113"/>
       <c r="B113"/>
       <c r="C113"/>
     </row>
-    <row r="114" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114"/>
       <c r="B114"/>
       <c r="C114"/>
     </row>
-    <row r="115" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115"/>
       <c r="B115"/>
       <c r="C115"/>
     </row>
-    <row r="116" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116"/>
       <c r="B116"/>
       <c r="C116"/>
     </row>
-    <row r="117" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117"/>
       <c r="B117"/>
       <c r="C117"/>
     </row>
-    <row r="118" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118"/>
       <c r="B118"/>
       <c r="C118"/>
     </row>
-    <row r="119" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119"/>
       <c r="B119"/>
       <c r="C119"/>
     </row>
-    <row r="120" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120"/>
       <c r="B120"/>
       <c r="C120"/>
     </row>
-    <row r="121" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121"/>
       <c r="B121"/>
       <c r="C121"/>
     </row>
-    <row r="122" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122"/>
       <c r="B122"/>
       <c r="C122"/>
     </row>
-    <row r="123" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123"/>
       <c r="B123"/>
       <c r="C123"/>
     </row>
-    <row r="124" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124"/>
       <c r="B124"/>
       <c r="C124"/>
     </row>
-    <row r="125" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125"/>
       <c r="B125"/>
       <c r="C125"/>
     </row>
-    <row r="126" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126"/>
       <c r="B126"/>
       <c r="C126"/>
     </row>
-    <row r="127" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127"/>
       <c r="B127"/>
       <c r="C127"/>
     </row>
-    <row r="128" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128"/>
       <c r="B128"/>
       <c r="C128"/>
     </row>
-    <row r="129" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129"/>
       <c r="B129"/>
       <c r="C129"/>
     </row>
-    <row r="130" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130"/>
       <c r="B130"/>
       <c r="C130"/>
     </row>
-    <row r="131" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131"/>
       <c r="B131"/>
       <c r="C131"/>
     </row>
-    <row r="132" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132"/>
       <c r="B132"/>
       <c r="C132"/>
     </row>
-    <row r="133" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133"/>
       <c r="B133"/>
       <c r="C133"/>
     </row>
-    <row r="134" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134"/>
       <c r="B134"/>
       <c r="C134"/>
     </row>
-    <row r="135" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135"/>
       <c r="B135"/>
       <c r="C135"/>
     </row>
-    <row r="136" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136"/>
       <c r="B136"/>
       <c r="C136"/>
     </row>
-    <row r="137" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137"/>
       <c r="B137"/>
       <c r="C137"/>
     </row>
-    <row r="138" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138"/>
       <c r="B138"/>
       <c r="C138"/>
     </row>
-    <row r="139" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139"/>
       <c r="B139"/>
       <c r="C139"/>
     </row>
-    <row r="140" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140"/>
       <c r="B140"/>
       <c r="C140"/>
     </row>
-    <row r="141" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141"/>
       <c r="B141"/>
       <c r="C141"/>
     </row>
-    <row r="142" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142"/>
       <c r="B142"/>
       <c r="C142"/>
     </row>
-    <row r="143" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143"/>
       <c r="B143"/>
       <c r="C143"/>
     </row>
-    <row r="144" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144"/>
       <c r="B144"/>
       <c r="C144"/>
     </row>
-    <row r="145" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145"/>
       <c r="B145"/>
       <c r="C145"/>
     </row>
-    <row r="146" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146"/>
       <c r="B146"/>
       <c r="C146"/>
     </row>
-    <row r="147" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147"/>
       <c r="B147"/>
       <c r="C147"/>
     </row>
-    <row r="148" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148"/>
       <c r="B148"/>
       <c r="C148"/>
     </row>
-    <row r="149" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149"/>
       <c r="B149"/>
       <c r="C149"/>
     </row>
-    <row r="150" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150"/>
       <c r="B150"/>
       <c r="C150"/>
     </row>
-    <row r="151" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151"/>
       <c r="B151"/>
       <c r="C151"/>
     </row>
-    <row r="152" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152"/>
       <c r="B152"/>
       <c r="C152"/>
     </row>
-    <row r="153" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153"/>
       <c r="B153"/>
       <c r="C153"/>
     </row>
-    <row r="154" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154"/>
       <c r="B154"/>
       <c r="C154"/>
     </row>
-    <row r="155" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155"/>
       <c r="B155"/>
       <c r="C155"/>
     </row>
-    <row r="156" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156"/>
       <c r="B156"/>
       <c r="C156"/>
     </row>
-    <row r="157" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157"/>
       <c r="B157"/>
       <c r="C157"/>
     </row>
-    <row r="158" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158"/>
       <c r="B158"/>
       <c r="C158"/>
     </row>
-    <row r="159" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159"/>
       <c r="B159"/>
       <c r="C159"/>
     </row>
-    <row r="160" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160"/>
       <c r="B160"/>
       <c r="C160"/>
     </row>
-    <row r="161" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161"/>
       <c r="B161"/>
       <c r="C161"/>
     </row>
-    <row r="162" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162"/>
       <c r="B162"/>
       <c r="C162"/>
     </row>
-    <row r="163" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163"/>
       <c r="B163"/>
       <c r="C163"/>
     </row>
-    <row r="164" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164"/>
       <c r="B164"/>
       <c r="C164"/>
     </row>
-    <row r="165" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165"/>
       <c r="B165"/>
       <c r="C165"/>
     </row>
-    <row r="166" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166"/>
       <c r="B166"/>
       <c r="C166"/>
     </row>
-    <row r="167" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167"/>
       <c r="B167"/>
       <c r="C167"/>
     </row>
-    <row r="168" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168"/>
       <c r="B168"/>
       <c r="C168"/>
     </row>
-    <row r="169" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169"/>
       <c r="B169"/>
       <c r="C169"/>
     </row>
-    <row r="170" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170"/>
       <c r="B170"/>
       <c r="C170"/>
     </row>
-    <row r="171" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171"/>
       <c r="B171"/>
       <c r="C171"/>
     </row>
-    <row r="172" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172"/>
       <c r="B172"/>
       <c r="C172"/>
     </row>
-    <row r="173" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173"/>
       <c r="B173"/>
       <c r="C173"/>
     </row>
-    <row r="174" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174"/>
       <c r="B174"/>
       <c r="C174"/>
     </row>
-    <row r="175" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175"/>
       <c r="B175"/>
       <c r="C175"/>
     </row>
-    <row r="176" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176"/>
       <c r="B176"/>
       <c r="C176"/>
     </row>
-    <row r="177" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177"/>
       <c r="B177"/>
       <c r="C177"/>
     </row>
-    <row r="178" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178"/>
       <c r="B178"/>
       <c r="C178"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
@@ -2534,13 +2536,14 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="A19:A36"/>
     <mergeCell ref="A38:A42"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>